<commit_message>
Added description to excelsheet
Signed-off-by: Deepesh Gurung <deepesh.gurung@technoforte.co.in>
</commit_message>
<xml_diff>
--- a/performance-test/MOSIP_TPS_Thread_setting_calculator-ID-Authentication.xlsx
+++ b/performance-test/MOSIP_TPS_Thread_setting_calculator-ID-Authentication.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PerfScripts\Release\Platform1.3.x\id-authentication\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\id-authentication\performance-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2600BC7-586F-4CC8-A047-FD954CCFD8F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67ABE90-333F-4229-B4A6-B8D89A4E6C52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00F0FE37-4E08-4BBA-8E9E-0C9A5473C445}"/>
   </bookViews>
   <sheets>
-    <sheet name="Esignet1.6.2" sheetId="2" r:id="rId1"/>
+    <sheet name="Calculator" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -22,6 +22,112 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Deepesh Gurung</author>
+  </authors>
+  <commentList>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{3C531CAA-56C7-4328-9131-AC83B070FF95}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Deepesh Gurung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+These will come from Performance test plan.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{824635CD-5815-4206-AEC2-B47CF71BF378}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Deepesh Gurung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This value is obtained from Jmeter results during previous executions and dry runs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{312B15C7-E052-4521-9F3E-A39592156D52}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Deepesh Gurung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Apply these values in Jmeter thread setting.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{116B6488-269F-4E8B-8B4A-12C73CCC770F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Deepesh Gurung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Apply this valie in Jmeter for "RampUp" variable under "user defined variables"</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -179,7 +285,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,6 +401,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -902,6 +1021,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -949,12 +1074,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1275,11 +1394,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66EF0A02-FD69-493C-AB91-7265D86F2CBF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66EF0A02-FD69-493C-AB91-7265D86F2CBF}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,25 +1417,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="H1" s="59" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="H1" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
     </row>
     <row r="2" spans="1:11" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="63"/>
       <c r="D2" s="45">
         <v>100</v>
       </c>
@@ -1329,11 +1448,11 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="56"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="58"/>
       <c r="D3" s="46">
         <f>$D$2*(SUM($E6:$E15)/($C$16*100))</f>
         <v>140</v>
@@ -1347,23 +1466,23 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="64"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="66"/>
       <c r="D4" s="44" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="2"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="65" t="s">
+      <c r="H4" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="67"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="69"/>
     </row>
     <row r="5" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
@@ -1399,7 +1518,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="52" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="31">
@@ -1438,7 +1557,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" s="49" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="34">
@@ -1474,7 +1593,7 @@
       <c r="K7" s="50"/>
     </row>
     <row r="8" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="53" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="34">
@@ -1507,12 +1626,12 @@
         <v>900</v>
       </c>
       <c r="J8" s="29"/>
-      <c r="K8" s="52" t="s">
+      <c r="K8" s="54" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="69" t="s">
+      <c r="A9" s="53" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="34">
@@ -1545,10 +1664,10 @@
         <v>1200</v>
       </c>
       <c r="J9" s="29"/>
-      <c r="K9" s="53"/>
+      <c r="K9" s="55"/>
     </row>
     <row r="10" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="69"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="34"/>
       <c r="C10" s="35"/>
       <c r="D10" s="36"/>
@@ -1573,10 +1692,10 @@
         <v>0</v>
       </c>
       <c r="J10" s="29"/>
-      <c r="K10" s="53"/>
+      <c r="K10" s="55"/>
     </row>
     <row r="11" spans="1:11" s="49" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="69"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="37"/>
       <c r="C11" s="38"/>
       <c r="D11" s="39"/>
@@ -1601,10 +1720,10 @@
         <v>0</v>
       </c>
       <c r="J11" s="29"/>
-      <c r="K11" s="54"/>
+      <c r="K11" s="56"/>
     </row>
     <row r="12" spans="1:11" s="49" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="69"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="37"/>
       <c r="C12" s="38"/>
       <c r="D12" s="39"/>
@@ -1634,7 +1753,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="69"/>
+      <c r="A13" s="53"/>
       <c r="B13" s="34"/>
       <c r="C13" s="35"/>
       <c r="D13" s="40"/>
@@ -1661,7 +1780,7 @@
       <c r="J13" s="30"/>
     </row>
     <row r="14" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="69"/>
+      <c r="A14" s="53"/>
       <c r="B14" s="34"/>
       <c r="C14" s="35"/>
       <c r="D14" s="36"/>
@@ -1763,5 +1882,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated readme file (#1613)
* resolved merge issue

Signed-off-by: Deepesh Gurung <deepesh.gurung@technoforte.co.in>

* Performance testing Release 1.3.x v0.3

Signed-off-by: Deepesh Gurung <deepesh.gurung@technoforte.co.in>

* Added description to excelsheet

Signed-off-by: Deepesh Gurung <deepesh.gurung@technoforte.co.in>

* Update Java 11 download link in README.md

Signed-off-by: DGuru <deepeshgurung@gmail.com>

---------

Signed-off-by: Deepesh Gurung <deepesh.gurung@technoforte.co.in>
Signed-off-by: DGuru <deepeshgurung@gmail.com>
Co-authored-by: Deepesh Gurung <deepesh.gurung@technoforte.co.in>
</commit_message>
<xml_diff>
--- a/performance-test/MOSIP_TPS_Thread_setting_calculator-ID-Authentication.xlsx
+++ b/performance-test/MOSIP_TPS_Thread_setting_calculator-ID-Authentication.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PerfScripts\Release\Platform1.3.x\id-authentication\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\id-authentication\performance-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2600BC7-586F-4CC8-A047-FD954CCFD8F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67ABE90-333F-4229-B4A6-B8D89A4E6C52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00F0FE37-4E08-4BBA-8E9E-0C9A5473C445}"/>
   </bookViews>
   <sheets>
-    <sheet name="Esignet1.6.2" sheetId="2" r:id="rId1"/>
+    <sheet name="Calculator" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -22,6 +22,112 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Deepesh Gurung</author>
+  </authors>
+  <commentList>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{3C531CAA-56C7-4328-9131-AC83B070FF95}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Deepesh Gurung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+These will come from Performance test plan.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{824635CD-5815-4206-AEC2-B47CF71BF378}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Deepesh Gurung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This value is obtained from Jmeter results during previous executions and dry runs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{312B15C7-E052-4521-9F3E-A39592156D52}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Deepesh Gurung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Apply these values in Jmeter thread setting.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{116B6488-269F-4E8B-8B4A-12C73CCC770F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Deepesh Gurung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Apply this valie in Jmeter for "RampUp" variable under "user defined variables"</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -179,7 +285,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,6 +401,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -902,6 +1021,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -949,12 +1074,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1275,11 +1394,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66EF0A02-FD69-493C-AB91-7265D86F2CBF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66EF0A02-FD69-493C-AB91-7265D86F2CBF}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,25 +1417,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="H1" s="59" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="H1" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
     </row>
     <row r="2" spans="1:11" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="63"/>
       <c r="D2" s="45">
         <v>100</v>
       </c>
@@ -1329,11 +1448,11 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="56"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="58"/>
       <c r="D3" s="46">
         <f>$D$2*(SUM($E6:$E15)/($C$16*100))</f>
         <v>140</v>
@@ -1347,23 +1466,23 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="64"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="66"/>
       <c r="D4" s="44" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="2"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="65" t="s">
+      <c r="H4" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="67"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="69"/>
     </row>
     <row r="5" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
@@ -1399,7 +1518,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="52" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="31">
@@ -1438,7 +1557,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" s="49" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="34">
@@ -1474,7 +1593,7 @@
       <c r="K7" s="50"/>
     </row>
     <row r="8" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="53" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="34">
@@ -1507,12 +1626,12 @@
         <v>900</v>
       </c>
       <c r="J8" s="29"/>
-      <c r="K8" s="52" t="s">
+      <c r="K8" s="54" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="69" t="s">
+      <c r="A9" s="53" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="34">
@@ -1545,10 +1664,10 @@
         <v>1200</v>
       </c>
       <c r="J9" s="29"/>
-      <c r="K9" s="53"/>
+      <c r="K9" s="55"/>
     </row>
     <row r="10" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="69"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="34"/>
       <c r="C10" s="35"/>
       <c r="D10" s="36"/>
@@ -1573,10 +1692,10 @@
         <v>0</v>
       </c>
       <c r="J10" s="29"/>
-      <c r="K10" s="53"/>
+      <c r="K10" s="55"/>
     </row>
     <row r="11" spans="1:11" s="49" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="69"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="37"/>
       <c r="C11" s="38"/>
       <c r="D11" s="39"/>
@@ -1601,10 +1720,10 @@
         <v>0</v>
       </c>
       <c r="J11" s="29"/>
-      <c r="K11" s="54"/>
+      <c r="K11" s="56"/>
     </row>
     <row r="12" spans="1:11" s="49" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="69"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="37"/>
       <c r="C12" s="38"/>
       <c r="D12" s="39"/>
@@ -1634,7 +1753,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="69"/>
+      <c r="A13" s="53"/>
       <c r="B13" s="34"/>
       <c r="C13" s="35"/>
       <c r="D13" s="40"/>
@@ -1661,7 +1780,7 @@
       <c r="J13" s="30"/>
     </row>
     <row r="14" spans="1:11" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="69"/>
+      <c r="A14" s="53"/>
       <c r="B14" s="34"/>
       <c r="C14" s="35"/>
       <c r="D14" s="36"/>
@@ -1763,5 +1882,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>